<commit_message>
Fixed density parameter values
</commit_message>
<xml_diff>
--- a/Elmer_files/ElmerSolver_Comparison.xlsx
+++ b/Elmer_files/ElmerSolver_Comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\ENGSCI700AB\Design-Automation-Optimisation-for-Multi-Material-3D-Printing\Elmer_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C38CCE-E89E-4F3D-B734-4152625B8D27}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0230F2-78B4-4DC2-A559-C908DB0B94E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="12750" windowHeight="10058" xr2:uid="{B6AA4588-B50D-46AC-8181-59F1726876DF}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="12750" windowHeight="10058" xr2:uid="{B6AA4588-B50D-46AC-8181-59F1726876DF}"/>
   </bookViews>
   <sheets>
     <sheet name="SolverOutput" sheetId="1" r:id="rId1"/>
@@ -1361,25 +1361,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1676.3732337481997</c:v>
+                  <c:v>53.011576271861571</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10505.692247538427</c:v>
+                  <c:v>332.21915898994905</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16763.732337482001</c:v>
+                  <c:v>530.11576271861566</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29409.834793313254</c:v>
+                  <c:v>930.02063556137239</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57644.429542202473</c:v>
+                  <c:v>1822.8769177445708</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105056.9224753843</c:v>
+                  <c:v>3322.1915898994907</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>95290.291256553945</c:v>
+                  <c:v>3013.3435927153887</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2641,13 +2641,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1676.3732337481997</c:v>
+                  <c:v>53.011576271861571</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1676.3732337481997</c:v>
+                  <c:v>53.011576271861571</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1676.3732337481997</c:v>
+                  <c:v>53.011576271861571</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5066,8 +5066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DCA0E69-817C-4EE7-B30D-E885100A269D}">
   <dimension ref="A1:S82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L17" zoomScale="122" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39:Q39"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5125,11 +5125,11 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
+      <c r="B4" s="2">
+        <v>1300</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1000</v>
       </c>
       <c r="F4" s="3"/>
       <c r="H4" s="3"/>
@@ -5262,11 +5262,11 @@
       </c>
       <c r="C14" s="5">
         <f>(B14^2/$B$7^2)*SQRT(($B$3*$B$8)/($B$4*$B$5*$B$6))/(2*PI())</f>
-        <v>16763.732337482001</v>
+        <v>530.11576271861566</v>
       </c>
       <c r="D14" s="1">
         <f>(B14^2/$B$7^2)*SQRT(($B$3*$B$9)/($B$4*$B$5*$B$6))/(2*PI())</f>
-        <v>1676.3732337481997</v>
+        <v>53.011576271861571</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -5281,11 +5281,11 @@
       </c>
       <c r="C15" s="5">
         <f>(B15^2/$B$7^2)*SQRT(($B$3*$B$8)/($B$4*$B$5*$B$6))/(2*PI())</f>
-        <v>105056.9224753843</v>
+        <v>3322.1915898994907</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" ref="D15:D19" si="0">(B15^2/$B$7^2)*SQRT(($B$3*$B$9)/($B$4*$B$5*$B$6))/(2*PI())</f>
-        <v>10505.692247538427</v>
+        <v>332.21915898994905</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -5300,11 +5300,11 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" ref="C16:C18" si="1">(B16^2/$B$7^2)*SQRT(($B$3*$B$8)/($B$4*$B$5*$B$6))/(2*PI())</f>
-        <v>294098.34793313255</v>
+        <v>9300.2063556137255</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>29409.834793313254</v>
+        <v>930.02063556137239</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -5317,11 +5317,11 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" si="1"/>
-        <v>576444.29542202479</v>
+        <v>18228.769177445709</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>57644.429542202473</v>
+        <v>1822.8769177445708</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.45">
@@ -5333,11 +5333,11 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" si="1"/>
-        <v>952902.91256553971</v>
+        <v>30133.435927153889</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>95290.291256553945</v>
+        <v>3013.3435927153887</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
@@ -5349,11 +5349,11 @@
       </c>
       <c r="C19" s="5">
         <f>(B19^2/$B$7^2)*SQRT(($B$3*$B$8)/($B$4*$B$5*$B$6))/(2*PI())</f>
-        <v>1423505.2053297732</v>
+        <v>45015.187099477436</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>142350.5205329773</v>
+        <v>4501.5187099477434</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
@@ -6243,7 +6243,7 @@
       </c>
       <c r="C45" s="2">
         <f>D14</f>
-        <v>1676.3732337481997</v>
+        <v>53.011576271861571</v>
       </c>
       <c r="D45" s="2">
         <f>SQRT(D24)/(2*PI())</f>
@@ -6302,7 +6302,7 @@
       </c>
       <c r="C46" s="2">
         <f>D15</f>
-        <v>10505.692247538427</v>
+        <v>332.21915898994905</v>
       </c>
       <c r="D46" s="2">
         <f>SQRT(E24)/(2*PI())</f>
@@ -6419,7 +6419,7 @@
       </c>
       <c r="C48" s="2">
         <f>C14</f>
-        <v>16763.732337482001</v>
+        <v>530.11576271861566</v>
       </c>
       <c r="D48" s="2">
         <f>SQRT(G24)/(2*PI())</f>
@@ -6478,7 +6478,7 @@
       </c>
       <c r="C49" s="2">
         <f>D16</f>
-        <v>29409.834793313254</v>
+        <v>930.02063556137239</v>
       </c>
       <c r="D49" s="2">
         <f>SQRT(H24)/(2*PI())</f>
@@ -6595,7 +6595,7 @@
       </c>
       <c r="C51" s="2">
         <f>D17</f>
-        <v>57644.429542202473</v>
+        <v>1822.8769177445708</v>
       </c>
       <c r="D51" s="2">
         <f>SQRT(J24)/(2*PI())</f>
@@ -6712,7 +6712,7 @@
       </c>
       <c r="C53" s="2">
         <f>C15</f>
-        <v>105056.9224753843</v>
+        <v>3322.1915898994907</v>
       </c>
       <c r="D53" s="2">
         <f>SQRT(L24)/(2*PI())</f>
@@ -6771,7 +6771,7 @@
       </c>
       <c r="C54" s="2">
         <f>D18</f>
-        <v>95290.291256553945</v>
+        <v>3013.3435927153887</v>
       </c>
       <c r="D54" s="2">
         <f>SQRT(M24)/(2*PI())</f>
@@ -6980,7 +6980,7 @@
       </c>
       <c r="H61" s="11">
         <f>C45</f>
-        <v>1676.3732337481997</v>
+        <v>53.011576271861571</v>
       </c>
       <c r="I61">
         <v>2164.9314026257775</v>
@@ -7017,7 +7017,7 @@
       </c>
       <c r="H62" s="11">
         <f>C46</f>
-        <v>10505.692247538427</v>
+        <v>332.21915898994905</v>
       </c>
       <c r="I62">
         <v>13521.3435019152</v>
@@ -7054,7 +7054,7 @@
       </c>
       <c r="H63" s="11">
         <f>C48</f>
-        <v>16763.732337482001</v>
+        <v>530.11576271861566</v>
       </c>
       <c r="I63">
         <v>16482.713231929214</v>
@@ -7091,7 +7091,7 @@
       </c>
       <c r="H64" s="11">
         <f>C49</f>
-        <v>29409.834793313254</v>
+        <v>930.02063556137239</v>
       </c>
       <c r="I64">
         <v>37865.503073717126</v>
@@ -7128,7 +7128,7 @@
       </c>
       <c r="H65" s="11">
         <f>C51</f>
-        <v>57644.429542202473</v>
+        <v>1822.8769177445708</v>
       </c>
       <c r="I65">
         <v>74310.889933580009</v>
@@ -7165,7 +7165,7 @@
       </c>
       <c r="H66" s="11">
         <f>C53</f>
-        <v>105056.9224753843</v>
+        <v>3322.1915898994907</v>
       </c>
       <c r="I66">
         <v>89887.254229566475</v>
@@ -7202,7 +7202,7 @@
       </c>
       <c r="H67" s="11">
         <f>C54</f>
-        <v>95290.291256553945</v>
+        <v>3013.3435927153887</v>
       </c>
       <c r="I67">
         <v>122975.92563195027</v>
@@ -7352,7 +7352,7 @@
       </c>
       <c r="D80" s="11">
         <f>H61</f>
-        <v>1676.3732337481997</v>
+        <v>53.011576271861571</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.45">
@@ -7367,7 +7367,7 @@
       </c>
       <c r="D81" s="11">
         <f>H61</f>
-        <v>1676.3732337481997</v>
+        <v>53.011576271861571</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.45">
@@ -7382,7 +7382,7 @@
       </c>
       <c r="D82" s="11">
         <f>H61</f>
-        <v>1676.3732337481997</v>
+        <v>53.011576271861571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>